<commit_message>
Updated the metadata for SDD data file
</commit_message>
<xml_diff>
--- a/Full data MW/MW_metadata.csv.xlsx
+++ b/Full data MW/MW_metadata.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdman\Desktop\Open-Data-MeadoWatch_2.0\Full data MW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajijohn/git/Open-Data-MeadoWatch/Full data MW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823C9EC2-C754-4042-8335-362F7C5940AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22245ABB-C9CB-DF4E-B035-71D487D1DA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="30940" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="137">
   <si>
     <t>Variable</t>
   </si>
@@ -426,22 +426,25 @@
     <t>Earliest day in the year with consistent snow cover in MM/DD/YYYY</t>
   </si>
   <si>
-    <t>Latest day in the year with consistent snow cover in MM/DD/YYYY</t>
-  </si>
-  <si>
     <t>Interval between snow appearance and dissapearance in days</t>
   </si>
   <si>
-    <t>minimum recorded soil temperature in the plot, degree celsius</t>
-  </si>
-  <si>
-    <t>date of snow dissapearance</t>
-  </si>
-  <si>
-    <t>comments on the SDD estimation, if needed</t>
-  </si>
-  <si>
-    <t>Predicted snow dissappearance date</t>
+    <t>Predicted snow dissappearance date, in DOY format</t>
+  </si>
+  <si>
+    <t>Minimum recorded soil temperature in the plot, degree celsius</t>
+  </si>
+  <si>
+    <t>Comments on the SDD estimation, if needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot name </t>
+  </si>
+  <si>
+    <t>Plot name</t>
+  </si>
+  <si>
+    <t>Latest day in the year with consistent snow cover in MM/DD/YYYY, generally the following year</t>
   </si>
 </sst>
 </file>
@@ -483,9 +486,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,21 +780,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" customWidth="1"/>
-    <col min="3" max="3" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.88671875" customWidth="1"/>
-    <col min="5" max="5" width="79.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="5" max="5" width="79.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -795,14 +807,14 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -815,11 +827,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -832,11 +844,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -849,11 +861,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -866,11 +878,11 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -883,11 +895,11 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -900,11 +912,11 @@
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -917,11 +929,11 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -931,11 +943,11 @@
       <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -945,11 +957,11 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -959,11 +971,11 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -973,11 +985,11 @@
       <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -987,11 +999,11 @@
       <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1001,11 +1013,11 @@
       <c r="D14" t="s">
         <v>16</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1015,11 +1027,11 @@
       <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="E15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1029,11 +1041,11 @@
       <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1043,11 +1055,11 @@
       <c r="D17" t="s">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1057,11 +1069,11 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1071,11 +1083,11 @@
       <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1085,11 +1097,11 @@
       <c r="D20" t="s">
         <v>16</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1099,11 +1111,11 @@
       <c r="D21" t="s">
         <v>16</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1113,11 +1125,11 @@
       <c r="D22" t="s">
         <v>16</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1127,11 +1139,11 @@
       <c r="D23" t="s">
         <v>16</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1141,11 +1153,11 @@
       <c r="D24" t="s">
         <v>16</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1155,11 +1167,11 @@
       <c r="D25" t="s">
         <v>16</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -1169,11 +1181,11 @@
       <c r="D26" t="s">
         <v>16</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -1183,11 +1195,11 @@
       <c r="D27" t="s">
         <v>36</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1197,11 +1209,11 @@
       <c r="D28" t="s">
         <v>36</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -1211,11 +1223,11 @@
       <c r="D29" t="s">
         <v>36</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>103</v>
       </c>
@@ -1225,11 +1237,11 @@
       <c r="D30" t="s">
         <v>36</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -1242,11 +1254,11 @@
       <c r="D31" t="s">
         <v>36</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -1256,11 +1268,11 @@
       <c r="D32" t="s">
         <v>36</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -1273,14 +1285,14 @@
       <c r="D33" t="s">
         <v>36</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="4" t="s">
         <v>112</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -1290,14 +1302,14 @@
       <c r="D34" t="s">
         <v>36</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="4" t="s">
         <v>114</v>
       </c>
       <c r="F34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -1307,14 +1319,14 @@
       <c r="D35" t="s">
         <v>36</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="4" t="s">
         <v>113</v>
       </c>
       <c r="F35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -1324,11 +1336,11 @@
       <c r="D36" t="s">
         <v>124</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1338,11 +1350,11 @@
       <c r="D37" t="s">
         <v>124</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -1352,11 +1364,11 @@
       <c r="D38" t="s">
         <v>124</v>
       </c>
-      <c r="E38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E38" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -1366,11 +1378,11 @@
       <c r="D39" t="s">
         <v>124</v>
       </c>
-      <c r="E39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E39" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -1380,11 +1392,11 @@
       <c r="D40" t="s">
         <v>124</v>
       </c>
-      <c r="E40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E40" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>117</v>
       </c>
@@ -1394,11 +1406,11 @@
       <c r="D41" t="s">
         <v>124</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -1411,11 +1423,11 @@
       <c r="D42" t="s">
         <v>124</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>119</v>
       </c>
@@ -1428,11 +1440,11 @@
       <c r="D43" t="s">
         <v>124</v>
       </c>
-      <c r="E43" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E43" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>120</v>
       </c>
@@ -1445,11 +1457,11 @@
       <c r="D44" t="s">
         <v>124</v>
       </c>
-      <c r="E44" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E44" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>121</v>
       </c>
@@ -1462,11 +1474,11 @@
       <c r="D45" t="s">
         <v>124</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>104</v>
       </c>
@@ -1479,11 +1491,11 @@
       <c r="D46" t="s">
         <v>124</v>
       </c>
-      <c r="E46" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E46" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>122</v>
       </c>
@@ -1493,11 +1505,11 @@
       <c r="D47" t="s">
         <v>124</v>
       </c>
-      <c r="E47" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E47" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>123</v>
       </c>
@@ -1510,8 +1522,8 @@
       <c r="D48" t="s">
         <v>124</v>
       </c>
-      <c r="E48" t="s">
-        <v>135</v>
+      <c r="E48" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1528,12 +1540,12 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1541,7 +1553,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1549,7 +1561,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1557,7 +1569,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1565,7 +1577,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1573,7 +1585,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1581,7 +1593,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1589,7 +1601,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1597,7 +1609,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1605,7 +1617,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1613,7 +1625,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -1621,7 +1633,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1629,7 +1641,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1637,7 +1649,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -1645,7 +1657,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1653,7 +1665,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1661,7 +1673,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1669,7 +1681,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>53</v>
       </c>

</xml_diff>